<commit_message>
Slight modifications has been done in the code. And 1 sheet is kept as open for testing purpose.
</commit_message>
<xml_diff>
--- a/1/review/design/design_review.xlsx
+++ b/1/review/design/design_review.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\My_Experiments\Perl\In_Excel\1\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\My_Experiments\SVNs\GitHub\Perl\trunk\1\review\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
     <t>hello how are you</t>
   </si>
   <si>
-    <t>Closed</t>
+    <t>Open</t>
   </si>
 </sst>
 </file>

</xml_diff>